<commit_message>
updates Test case doc
</commit_message>
<xml_diff>
--- a/TestCases/TestCases.xlsx
+++ b/TestCases/TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace_Bw6\GitRepo\Employee_Details\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6641400-8BF8-4450-826D-0FB7C33112F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF88E43-23DD-4F66-97CE-9307F08F9FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FA7518AD-BAA6-4064-84C9-F8ACC843706A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{FA7518AD-BAA6-4064-84C9-F8ACC843706A}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee_Personal" sheetId="1" r:id="rId1"/>
@@ -381,6 +381,59 @@
     <t>Date-of-joining format should be yyyy-mm-dd, should not contain sring</t>
   </si>
   <si>
+    <t>Valid Json Req</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Invalid JSON:
+	  {
+		"EmpCode": "1001",
+		"EmpName": "Shiva Kollati",
+		"EmailID": "shivaK@eniquesolutions.com",
+		"Alt_EmailID": "shivaK@gmail.com",
+		"PhoneNo": 9897867578,
+		"DOB": "2022-11-10s",
+		"MaritalStatus": "single",
+		"Age": 28,
+		"AadhaarNo": 87986765ss,
+		"PAN_Number": "RJCTY5664A"
+	  }</t>
+  </si>
+  <si>
+    <t>AadhaarNo should not conatin string</t>
+  </si>
+  <si>
+    <t>Invalid JSON:
+{
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"Title": "Senior Integration Consutant",
+		"CurrentSal": 40000,
+		"lastModifiedDate": "10-11-2022T11:16:4sd"
+	  }</t>
+  </si>
+  <si>
+    <t>LastModifiedDate format should be yyyy-MM-ddTHH:mm:SS.ssZ
+should not contain String</t>
+  </si>
+  <si>
+    <t>personal Aadhaarno should not conatin string</t>
+  </si>
+  <si>
+    <t>personal DOB should be of format yyyy-MM-DD</t>
+  </si>
+  <si>
+    <t>personal EmailID should be In a format name@domain.com</t>
+  </si>
+  <si>
+    <t>Professional Date of Joining should be of format yyyy-MM-DD</t>
+  </si>
+  <si>
+    <t>Emp_SalTitle req is not present</t>
+  </si>
+  <si>
     <t>validJSON:	{
 	  "EmpPersonal": {
 		"EmpCode": "",
@@ -439,50 +492,9 @@
 		"PolicyNumber": "PN005/ES8564/004",
 		"PolicyType": "Premium",
 		"SumInsured": 50000,
-		"ValidTill": "2024-11-10s"
+		"ValidTill": "2024-11-10"
 	  }
 	}</t>
-  </si>
-  <si>
-    <t>Valid Json Req</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>Invalid JSON:
-	  {
-		"EmpCode": "1001",
-		"EmpName": "Shiva Kollati",
-		"EmailID": "shivaK@eniquesolutions.com",
-		"Alt_EmailID": "shivaK@gmail.com",
-		"PhoneNo": 9897867578,
-		"DOB": "2022-11-10s",
-		"MaritalStatus": "single",
-		"Age": 28,
-		"AadhaarNo": 87986765ss,
-		"PAN_Number": "RJCTY5664A"
-	  }</t>
-  </si>
-  <si>
-    <t>AadhaarNo should not conatin string</t>
-  </si>
-  <si>
-    <t>Invalid JSON:
-{
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"Title": "Senior Integration Consutant",
-		"CurrentSal": 40000,
-		"lastModifiedDate": "10-11-2022T11:16:4sd"
-	  }</t>
-  </si>
-  <si>
-    <t>LastModifiedDate format should be yyyy-MM-ddTHH:mm:SS.ssZ
-should not contain String</t>
-  </si>
-  <si>
-    <t>personal Aadhaarno should not conatin string</t>
   </si>
   <si>
     <t>InvalidJSON:	{
@@ -543,22 +555,141 @@
 		"PolicyNumber": "PN005/ES8564/004",
 		"PolicyType": "Premium",
 		"SumInsured": 50000,
-		"ValidTill": "2024-11-10s"
+		"ValidTill": "2024-11-10"
 	  }
 	}</t>
   </si>
   <si>
-    <t>validJSON:	{
+    <t>InvalidJSON:	{
 	  "EmpPersonal": {
 		"EmpCode": "",
 		"EmpName": "Shiva Kollati",
 		"EmailID": "shivaK@eniquesolutions.com",
 		"Alt_EmailID": "shivaK@gmail.com",
 		"PhoneNo": 9897867578,
-		"DOB": "10-11-2022",
+		"DOB": "2022-11-12",
 		"MaritalStatus": "single",
 		"Age": 28,
-		"AadhaarNo": 879867656678ss,
+		"AadhaarNo": 879867656678,
+		"PAN_Number": "RJCTY5664A"
+	  },
+	  "Employee_Prof": {
+		"EmpCode": "",
+		"Department": "Tibco",
+		"Reporting-To": "Nagendra",
+		"Seating-Location": "4th Floor",
+		"Location": "Hyderabad",
+		"Title": "Asc Consutant",
+		"Date-of-joining": "10-11-2022",
+		"Employee-status": "Active",
+		"Employee-type": "Permanent",
+		"Role": "Team member",
+		"Experience": "11 months"
+	  },
+	  "Employee_Address": {
+		"EmpCode": "",
+		"AddressLine1": "Jayabheri Pine Valley",
+		"AddressLine2": "Gachibowli",
+		"Landmark": "care Hospital",
+		"City": "Hyderabad",
+		"State": "Tealangana",
+		"ZipCode": "500032"
+	  },
+	  "Emp_OrgDetails": {
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"OrganizationName": "Enique Solutions Pvt. Ltd.",
+		"CompanyHQ": "Hyderabad",
+		"CompanyPhNo": 8796056748,
+		"OrgAddress": "Gachibowli",
+		"DirectorName": "PR"
+	  },
+	  "Emp_Insurence": {
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"OrgName": "Enique Solutions Pvt. Ltd.",
+		"PolicyNumber": "PN005/ES8564/004",
+		"PolicyType": "Premium",
+		"SumInsured": 50000,
+		"ValidTill": "2024-11-10"
+	  }
+	}</t>
+  </si>
+  <si>
+    <t>InvalidJSON:	{
+	  "EmpPersonal": {
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"EmailID": "shivaK@eniquesolutions.com",
+		"Alt_EmailID": "shivaK@gmail.com",
+		"PhoneNo": 9897867578,
+		"DOB": "2022-11-12",
+		"MaritalStatus": "single",
+		"Age": 28,
+		"AadhaarNo": 879867656678,
+		"PAN_Number": "RJCTY5664A"
+	  },
+	  "Employee_Prof": {
+		"EmpCode": "",
+		"Department": "Tibco",
+		"Reporting-To": "Nagendra",
+		"Seating-Location": "4th Floor",
+		"Location": "Hyderabad",
+		"Title": "Asc Consutant",
+		"Date-of-joining": "10-11-2022",
+		"Employee-status": "Active",
+		"Employee-type": "Permanent",
+		"Role": "Team member",
+		"Experience": "11 months"
+	  },
+	  "Employee_Address": {
+		"EmpCode": "",
+		"AddressLine1": "Jayabheri Pine Valley",
+		"AddressLine2": "Gachibowli",
+		"Landmark": "care Hospital",
+		"City": "Hyderabad",
+		"State": "Tealangana",
+		"ZipCode": "500032"
+	  },
+	  "Emp_OrgDetails": {
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"OrganizationName": "Enique Solutions Pvt. Ltd.",
+		"CompanyHQ": "Hyderabad",
+		"CompanyPhNo": 8796056748,
+		"OrgAddress": "Gachibowli",
+		"DirectorName": "PR"
+	  },
+	  "Emp_SalTitle": {
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"Title": "Senior Integration Consutant",
+		"CurrentSal": 40000,
+		"lastModifiedDate": "2022-11-10T11:16:47.990Z"
+	  },
+	  "Emp_Insurence": {
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"OrgName": "Enique Solutions Pvt. Ltd.",
+		"PolicyNumber": "PN005/ES8564/004",
+		"PolicyType": "Premium",
+		"SumInsured": 50000,
+		"ValidTill": "2024-11-10"
+	  }
+	}</t>
+  </si>
+  <si>
+    <t>InvalidJSON:	{
+	  "EmpPersonal": {
+		"EmpCode": "",
+		"EmpName": "Shiva Kollati",
+		"EmailID": "shivaK.com",
+		"Alt_EmailID": "shivaK@gmail.com",
+		"PhoneNo": 9897867578,
+		"DOB": "2022-11-12",
+		"MaritalStatus": "single",
+		"Age": 28,
+		"AadhaarNo": 879867656678,
 		"PAN_Number": "RJCTY5664A"
 	  },
 	  "Employee_Prof": {
@@ -606,25 +737,22 @@
 		"PolicyNumber": "PN005/ES8564/004",
 		"PolicyType": "Premium",
 		"SumInsured": 50000,
-		"ValidTill": "2024-11-10s"
+		"ValidTill": "2024-11-10"
 	  }
 	}</t>
   </si>
   <si>
-    <t>personal DOB should be of format yyyy-MM-DD</t>
-  </si>
-  <si>
-    <t>validJSON:	{
+    <t>InvalidJSON:	{
 	  "EmpPersonal": {
 		"EmpCode": "",
 		"EmpName": "Shiva Kollati",
-		"EmailID": "shivaK.com",
+		"EmailID": "shivaK@eniquesolutions.com",
 		"Alt_EmailID": "shivaK@gmail.com",
 		"PhoneNo": 9897867578,
-		"DOB": "2022-11-12",
+		"DOB": "10-11-2022",
 		"MaritalStatus": "single",
 		"Age": 28,
-		"AadhaarNo": 879867656678,
+		"AadhaarNo": 879867656678ss,
 		"PAN_Number": "RJCTY5664A"
 	  },
 	  "Employee_Prof": {
@@ -672,135 +800,7 @@
 		"PolicyNumber": "PN005/ES8564/004",
 		"PolicyType": "Premium",
 		"SumInsured": 50000,
-		"ValidTill": "2024-11-10s"
-	  }
-	}</t>
-  </si>
-  <si>
-    <t>personal EmailID should be In a format name@domain.com</t>
-  </si>
-  <si>
-    <t>validJSON:	{
-	  "EmpPersonal": {
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"EmailID": "shivaK@eniquesolutions.com",
-		"Alt_EmailID": "shivaK@gmail.com",
-		"PhoneNo": 9897867578,
-		"DOB": "2022-11-12",
-		"MaritalStatus": "single",
-		"Age": 28,
-		"AadhaarNo": 879867656678,
-		"PAN_Number": "RJCTY5664A"
-	  },
-	  "Employee_Prof": {
-		"EmpCode": "",
-		"Department": "Tibco",
-		"Reporting-To": "Nagendra",
-		"Seating-Location": "4th Floor",
-		"Location": "Hyderabad",
-		"Title": "Asc Consutant",
-		"Date-of-joining": "10-11-2022",
-		"Employee-status": "Active",
-		"Employee-type": "Permanent",
-		"Role": "Team member",
-		"Experience": "11 months"
-	  },
-	  "Employee_Address": {
-		"EmpCode": "",
-		"AddressLine1": "Jayabheri Pine Valley",
-		"AddressLine2": "Gachibowli",
-		"Landmark": "care Hospital",
-		"City": "Hyderabad",
-		"State": "Tealangana",
-		"ZipCode": "500032"
-	  },
-	  "Emp_OrgDetails": {
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"OrganizationName": "Enique Solutions Pvt. Ltd.",
-		"CompanyHQ": "Hyderabad",
-		"CompanyPhNo": 8796056748,
-		"OrgAddress": "Gachibowli",
-		"DirectorName": "PR"
-	  },
-	  "Emp_SalTitle": {
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"Title": "Senior Integration Consutant",
-		"CurrentSal": 40000,
-		"lastModifiedDate": "2022-11-10T11:16:47.990Z"
-	  },
-	  "Emp_Insurence": {
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"OrgName": "Enique Solutions Pvt. Ltd.",
-		"PolicyNumber": "PN005/ES8564/004",
-		"PolicyType": "Premium",
-		"SumInsured": 50000,
-		"ValidTill": "2024-11-10s"
-	  }
-	}</t>
-  </si>
-  <si>
-    <t>Professional Date of Joining should be of format yyyy-MM-DD</t>
-  </si>
-  <si>
-    <t>Emp_SalTitle req is not present</t>
-  </si>
-  <si>
-    <t>validJSON:	{
-	  "EmpPersonal": {
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"EmailID": "shivaK@eniquesolutions.com",
-		"Alt_EmailID": "shivaK@gmail.com",
-		"PhoneNo": 9897867578,
-		"DOB": "2022-11-12",
-		"MaritalStatus": "single",
-		"Age": 28,
-		"AadhaarNo": 879867656678,
-		"PAN_Number": "RJCTY5664A"
-	  },
-	  "Employee_Prof": {
-		"EmpCode": "",
-		"Department": "Tibco",
-		"Reporting-To": "Nagendra",
-		"Seating-Location": "4th Floor",
-		"Location": "Hyderabad",
-		"Title": "Asc Consutant",
-		"Date-of-joining": "10-11-2022",
-		"Employee-status": "Active",
-		"Employee-type": "Permanent",
-		"Role": "Team member",
-		"Experience": "11 months"
-	  },
-	  "Employee_Address": {
-		"EmpCode": "",
-		"AddressLine1": "Jayabheri Pine Valley",
-		"AddressLine2": "Gachibowli",
-		"Landmark": "care Hospital",
-		"City": "Hyderabad",
-		"State": "Tealangana",
-		"ZipCode": "500032"
-	  },
-	  "Emp_OrgDetails": {
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"OrganizationName": "Enique Solutions Pvt. Ltd.",
-		"CompanyHQ": "Hyderabad",
-		"CompanyPhNo": 8796056748,
-		"OrgAddress": "Gachibowli",
-		"DirectorName": "PR"
-	  },
-	  "Emp_Insurence": {
-		"EmpCode": "",
-		"EmpName": "Shiva Kollati",
-		"OrgName": "Enique Solutions Pvt. Ltd.",
-		"PolicyNumber": "PN005/ES8564/004",
-		"PolicyType": "Premium",
-		"SumInsured": 50000,
-		"ValidTill": "2024-11-10s"
+		"ValidTill": "2024-11-10"
 	  }
 	}</t>
   </si>
@@ -1184,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379B2B1C-AEEF-4F97-B1BE-B050B28C3378}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1319,10 +1319,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1684,10 +1684,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -1809,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4776FA-4079-4B42-B559-A0EC0931673D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1845,13 +1845,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1862,10 +1862,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -1879,10 +1879,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -1896,10 +1896,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -1913,10 +1913,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -1930,10 +1930,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -1941,6 +1941,12 @@
       <c r="E7" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>